<commit_message>
December 2022 last updates
</commit_message>
<xml_diff>
--- a/quantifyVagusNerve/Data/Supporting Files/Biological Information/Bio_info.xlsx
+++ b/quantifyVagusNerve/Data/Supporting Files/Biological Information/Bio_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja\Documents\GitHub\spatial-neuro\quantifyVagusNerve\Data\Supporting Files\Biological Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634A34BB-62CF-4FE9-AC48-40A088DF5AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8155C3-0FB1-458D-8E48-04F5F8299FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="84">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -263,6 +263,15 @@
   </si>
   <si>
     <t>Image_ID</t>
+  </si>
+  <si>
+    <t>Nerve Type</t>
+  </si>
+  <si>
+    <t>Cervical Vagus</t>
+  </si>
+  <si>
+    <t>Abdominal Vagus</t>
   </si>
 </sst>
 </file>
@@ -319,10 +328,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,11 +629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,9 +642,10 @@
     <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -656,8 +667,11 @@
       <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -679,8 +693,11 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -702,8 +719,11 @@
       <c r="G3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -725,8 +745,11 @@
       <c r="G4" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -748,8 +771,11 @@
       <c r="G5" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -771,8 +797,11 @@
       <c r="G6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -794,8 +823,11 @@
       <c r="G7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -817,8 +849,11 @@
       <c r="G8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -840,8 +875,11 @@
       <c r="G9" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -863,8 +901,11 @@
       <c r="G10" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -886,8 +927,11 @@
       <c r="G11" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -909,8 +953,11 @@
       <c r="G12" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -932,8 +979,11 @@
       <c r="G13" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -955,8 +1005,11 @@
       <c r="G14" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -978,8 +1031,11 @@
       <c r="G15" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1001,8 +1057,11 @@
       <c r="G16" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1024,8 +1083,11 @@
       <c r="G17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1047,8 +1109,11 @@
       <c r="G18" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1070,8 +1135,11 @@
       <c r="G19" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1093,8 +1161,11 @@
       <c r="G20" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1116,8 +1187,11 @@
       <c r="G21" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1139,8 +1213,11 @@
       <c r="G22" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1162,8 +1239,11 @@
       <c r="G23" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1185,8 +1265,11 @@
       <c r="G24" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1208,8 +1291,11 @@
       <c r="G25" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1231,8 +1317,11 @@
       <c r="G26" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1254,8 +1343,11 @@
       <c r="G27" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1277,8 +1369,11 @@
       <c r="G28" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1300,8 +1395,11 @@
       <c r="G29" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1322,6 +1420,9 @@
       </c>
       <c r="G30" s="1">
         <v>29</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>